<commit_message>
Added .gitignore for schematic subdir to exclude temp. Eagle files. Updated BOM. Added Eagle BOM textfile. Updated schematic. Added Debug interface.
</commit_message>
<xml_diff>
--- a/Hardware/BOM.xlsx
+++ b/Hardware/BOM.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="70">
   <si>
     <t>CANWakeUp BOM</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Microcontroller</t>
   </si>
   <si>
-    <t>STM32F103C8T6</t>
-  </si>
-  <si>
     <t>Price</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>Switch</t>
   </si>
   <si>
-    <t>TJA1050</t>
-  </si>
-  <si>
     <t>Reichelt</t>
   </si>
   <si>
@@ -81,10 +75,160 @@
     <t>Texas Instruments LM1117MP-3.3</t>
   </si>
   <si>
-    <t>Power LED</t>
-  </si>
-  <si>
-    <t>TX LED</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>IC4</t>
+  </si>
+  <si>
+    <t>IC5</t>
+  </si>
+  <si>
+    <t>IC1</t>
+  </si>
+  <si>
+    <t>DA1</t>
+  </si>
+  <si>
+    <t>SWITCH</t>
+  </si>
+  <si>
+    <t>LED1</t>
+  </si>
+  <si>
+    <t>LED2</t>
+  </si>
+  <si>
+    <t>TX LED Green</t>
+  </si>
+  <si>
+    <t>Power LED Red</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>Resistors</t>
+  </si>
+  <si>
+    <t>Capacitors</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>C14</t>
+  </si>
+  <si>
+    <t>R0805</t>
+  </si>
+  <si>
+    <t>C0805</t>
+  </si>
+  <si>
+    <t>Kingbright LED, 3 mm, bedrahtet, rot, 5 mcd, 60°</t>
+  </si>
+  <si>
+    <t>Kingbright LED, 3 mm, bedrahtet, grün, 18 mcd, 60°</t>
+  </si>
+  <si>
+    <t>Summe/Muster</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>XTAL</t>
+  </si>
+  <si>
+    <t>SMD-Widerstand, 0805, 68 Ohm, 125 mW, 1%</t>
+  </si>
+  <si>
+    <t>SMD-Widerstand, 0805, 10 kOhm, 125 mW, 1%</t>
+  </si>
+  <si>
+    <t>SMD-Widerstand, 0805, 56 Ohm, 125 mW, 1%</t>
+  </si>
+  <si>
+    <t>SMD-Widerstand, 0805, 390 Ohm, 125 mW, 1%</t>
+  </si>
+  <si>
+    <t>SMD-Quarz, Grundton, 8,000000 MHz</t>
+  </si>
+  <si>
+    <t>TJA1050 Schnittstellen-IC, CAN, SOT-96-1</t>
+  </si>
+  <si>
+    <t>SMD-Vielschicht-Keramikkondensator 10N, 10%</t>
+  </si>
+  <si>
+    <t>SMD-Kerko, 0805, 1 µF, 10 V, 10%, MLCC</t>
+  </si>
+  <si>
+    <t>STM32F103C8T6 32-Bit Flash-Microcontroller CORTEX-M3,LQFP48</t>
+  </si>
+  <si>
+    <t>SMD-Vielschicht-Keramikkondensator 100N, 10%</t>
+  </si>
+  <si>
+    <t>SMD-Vielschicht-Keramikkondensator 22P, 5%</t>
+  </si>
+  <si>
+    <t>Schiebeschalter-Miniatur, Lötanschluss, 2x UM sw</t>
   </si>
 </sst>
 </file>
@@ -94,7 +238,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +254,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -119,11 +271,60 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -132,18 +333,340 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="8">
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -159,14 +682,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="B5:F12" totalsRowShown="0">
-  <autoFilter ref="B5:F12"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Domain"/>
-    <tableColumn id="2" name="Name"/>
-    <tableColumn id="3" name="Device"/>
-    <tableColumn id="4" name="Link"/>
-    <tableColumn id="5" name="Price" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabelle3" displayName="Tabelle3" ref="B5:G34" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="B5:G34"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Domain" dataDxfId="7"/>
+    <tableColumn id="2" name="ID" dataDxfId="6"/>
+    <tableColumn id="3" name="Name" dataDxfId="5"/>
+    <tableColumn id="4" name="Device" dataDxfId="4"/>
+    <tableColumn id="5" name="Link" dataDxfId="3"/>
+    <tableColumn id="6" name="Price" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -435,127 +959,628 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F12"/>
+  <dimension ref="B3:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" customWidth="1"/>
-    <col min="4" max="4" width="36.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="10"/>
+      <c r="C7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="13">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="13">
+        <v>3.99</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="13">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="C10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>21</v>
+      <c r="E10" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="13">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="10"/>
+      <c r="C11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="10"/>
+      <c r="C12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="10"/>
+      <c r="C13" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="13">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="13">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="10"/>
+      <c r="C15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="13">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="10"/>
+      <c r="C16" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="13">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="10"/>
+      <c r="C17" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="13">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="10"/>
+      <c r="C18" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="13">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="10"/>
+      <c r="C19" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="13">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="10"/>
+      <c r="C20" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="13">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="13">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="10"/>
+      <c r="C22" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="13">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="10"/>
+      <c r="C23" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="13">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="10"/>
+      <c r="C24" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="13">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="10"/>
+      <c r="C25" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="13">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="10"/>
+      <c r="C26" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="13">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="10"/>
+      <c r="C27" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="13">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="10"/>
+      <c r="C28" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="13">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="10"/>
+      <c r="C29" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="13">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="10"/>
+      <c r="C30" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="13">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="10"/>
+      <c r="C31" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="10"/>
+      <c r="C32" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="10"/>
+      <c r="C33" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="13">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="10"/>
+      <c r="C34" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" s="13">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="2">
+        <f>SUM(G:G)</f>
+        <v>7.8099999999999978</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1"/>
-    <hyperlink ref="E7" r:id="rId2"/>
-    <hyperlink ref="E8" r:id="rId3"/>
+    <hyperlink ref="F6" r:id="rId1"/>
+    <hyperlink ref="F7" r:id="rId2"/>
+    <hyperlink ref="F8" r:id="rId3"/>
+    <hyperlink ref="F12" r:id="rId4"/>
+    <hyperlink ref="F11" r:id="rId5"/>
+    <hyperlink ref="F18" r:id="rId6"/>
+    <hyperlink ref="F19" r:id="rId7"/>
+    <hyperlink ref="F20" r:id="rId8"/>
+    <hyperlink ref="F14" r:id="rId9"/>
+    <hyperlink ref="F15" r:id="rId10"/>
+    <hyperlink ref="F17" r:id="rId11"/>
+    <hyperlink ref="F16" r:id="rId12"/>
+    <hyperlink ref="F13" r:id="rId13"/>
+    <hyperlink ref="F9" r:id="rId14"/>
+    <hyperlink ref="F21" r:id="rId15"/>
+    <hyperlink ref="F22" r:id="rId16"/>
+    <hyperlink ref="F23" r:id="rId17"/>
+    <hyperlink ref="F24" r:id="rId18"/>
+    <hyperlink ref="F25" r:id="rId19"/>
+    <hyperlink ref="F26" r:id="rId20"/>
+    <hyperlink ref="F27" r:id="rId21"/>
+    <hyperlink ref="F28" r:id="rId22"/>
+    <hyperlink ref="F29" r:id="rId23"/>
+    <hyperlink ref="F31" r:id="rId24"/>
+    <hyperlink ref="F32" r:id="rId25"/>
+    <hyperlink ref="F30" r:id="rId26"/>
+    <hyperlink ref="F33" r:id="rId27"/>
+    <hyperlink ref="F34" r:id="rId28"/>
+    <hyperlink ref="F10" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId30"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId31"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished board layout. First order at seeedstudio.com
</commit_message>
<xml_diff>
--- a/Hardware/BOM.xlsx
+++ b/Hardware/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="71">
   <si>
     <t xml:space="preserve">CANWakeUp BOM</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t xml:space="preserve">Kingbright LED SMD 0805, green, 12mcd, 120°</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSUB-9</t>
   </si>
   <si>
     <t xml:space="preserve">Q1</t>
@@ -509,8 +512,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle3" displayName="Tabelle3" ref="B5:G34" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="B5:G34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle3" displayName="Tabelle3" ref="B5:G35" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="B5:G35"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Domain"/>
     <tableColumn id="2" name="ID"/>
@@ -527,10 +530,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:G38"/>
+  <dimension ref="B3:G39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -704,56 +707,52 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="10"/>
       <c r="C13" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="13" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="10"/>
+      <c r="C14" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="D14" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="13" t="n">
+      <c r="E14" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="13" t="n">
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="11" t="s">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="C15" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="D15" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="13" t="n">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="10"/>
-      <c r="C15" s="11" t="s">
+      <c r="E15" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="14" t="s">
         <v>11</v>
       </c>
       <c r="G15" s="13" t="n">
@@ -763,13 +762,13 @@
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="10"/>
       <c r="C16" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="11" t="s">
         <v>42</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>11</v>
@@ -781,13 +780,13 @@
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="10"/>
       <c r="C17" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>44</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>45</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>11</v>
@@ -799,15 +798,15 @@
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="10"/>
       <c r="C18" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="12" t="s">
         <v>11</v>
       </c>
       <c r="G18" s="13" t="n">
@@ -820,10 +819,10 @@
         <v>47</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F19" s="14" t="s">
         <v>11</v>
@@ -838,10 +837,10 @@
         <v>48</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F20" s="14" t="s">
         <v>11</v>
@@ -851,35 +850,35 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="10"/>
+      <c r="C21" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="D21" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="13" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="C22" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="13" t="n">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="10"/>
-      <c r="C22" s="11" t="s">
+      <c r="D22" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="11" t="s">
         <v>53</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>52</v>
       </c>
       <c r="F22" s="14" t="s">
         <v>11</v>
@@ -894,10 +893,10 @@
         <v>54</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>11</v>
@@ -912,10 +911,10 @@
         <v>55</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F24" s="14" t="s">
         <v>11</v>
@@ -930,10 +929,10 @@
         <v>56</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F25" s="14" t="s">
         <v>11</v>
@@ -948,10 +947,10 @@
         <v>57</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F26" s="14" t="s">
         <v>11</v>
@@ -966,10 +965,10 @@
         <v>58</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F27" s="14" t="s">
         <v>11</v>
@@ -984,10 +983,10 @@
         <v>59</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F28" s="14" t="s">
         <v>11</v>
@@ -1002,10 +1001,10 @@
         <v>60</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F29" s="14" t="s">
         <v>11</v>
@@ -1020,10 +1019,10 @@
         <v>61</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="F30" s="14" t="s">
         <v>11</v>
@@ -1035,31 +1034,31 @@
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="10"/>
       <c r="C31" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E31" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>64</v>
-      </c>
       <c r="F31" s="14" t="s">
         <v>11</v>
       </c>
       <c r="G31" s="13" t="n">
-        <v>0.07</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="10"/>
       <c r="C32" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" s="11" t="s">
         <v>65</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>64</v>
       </c>
       <c r="F32" s="14" t="s">
         <v>11</v>
@@ -1074,28 +1073,28 @@
         <v>66</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F33" s="14" t="s">
         <v>11</v>
       </c>
       <c r="G33" s="13" t="n">
-        <v>0.02</v>
+        <v>0.07</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="10"/>
       <c r="C34" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E34" s="11" t="s">
         <v>68</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E34" s="11" t="s">
-        <v>67</v>
       </c>
       <c r="F34" s="14" t="s">
         <v>11</v>
@@ -1104,17 +1103,35 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="1" t="s">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="10"/>
+      <c r="C35" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C36" s="2" t="n">
+      <c r="D35" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="13" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C37" s="2" t="n">
         <f aca="false">SUM(G:G)</f>
-        <v>7.87</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>8.27</v>
+      </c>
+    </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" display="Reichelt"/>
@@ -1146,6 +1163,7 @@
     <hyperlink ref="F32" r:id="rId27" display="Reichelt"/>
     <hyperlink ref="F33" r:id="rId28" display="Reichelt"/>
     <hyperlink ref="F34" r:id="rId29" display="Reichelt"/>
+    <hyperlink ref="F35" r:id="rId30" display="Reichelt"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1155,7 +1173,7 @@
     <oddFooter/>
   </headerFooter>
   <tableParts>
-    <tablePart r:id="rId30"/>
+    <tablePart r:id="rId31"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New version. Added Eagle BOM (.csv) file.
</commit_message>
<xml_diff>
--- a/Hardware/BOM.xlsx
+++ b/Hardware/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="73">
   <si>
     <t xml:space="preserve">CANWakeUp BOM</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t xml:space="preserve">DSUB-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSUB-9 Stecker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D-SUB-Stecker, 9-polig, gewinkelt, RM 2,77</t>
   </si>
   <si>
     <t xml:space="preserve">Q1</t>
@@ -377,7 +383,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -431,6 +437,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -530,13 +540,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:G39"/>
+  <dimension ref="B3:G37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.14"/>
@@ -548,12 +558,12 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
@@ -573,7 +583,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
@@ -593,7 +603,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="10"/>
       <c r="C7" s="11" t="s">
         <v>12</v>
@@ -611,7 +621,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="10" t="s">
         <v>15</v>
       </c>
@@ -631,7 +641,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="10" t="s">
         <v>19</v>
       </c>
@@ -651,7 +661,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="10" t="s">
         <v>23</v>
       </c>
@@ -712,8 +722,12 @@
       <c r="C13" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
+      <c r="D13" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>35</v>
+      </c>
       <c r="F13" s="12" t="s">
         <v>11</v>
       </c>
@@ -721,54 +735,54 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="10"/>
       <c r="C14" s="11" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G14" s="13" t="n">
         <v>0.25</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G15" s="13" t="n">
         <v>0.03</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="10"/>
       <c r="C16" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="11" t="s">
-        <v>39</v>
-      </c>
       <c r="E16" s="11" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>11</v>
@@ -777,16 +791,16 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="10"/>
       <c r="C17" s="11" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>11</v>
@@ -795,16 +809,16 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="10"/>
       <c r="C18" s="11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>11</v>
@@ -813,325 +827,323 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="10"/>
       <c r="C19" s="11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G19" s="13" t="n">
         <v>0.03</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="10"/>
       <c r="C20" s="11" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G20" s="13" t="n">
         <v>0.03</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="10"/>
       <c r="C21" s="11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G21" s="13" t="n">
         <v>0.03</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="10" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F22" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G22" s="13" t="n">
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="10"/>
       <c r="C23" s="11" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G23" s="13" t="n">
         <v>0.02</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="10"/>
       <c r="C24" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G24" s="13" t="n">
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="10"/>
       <c r="C25" s="11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G25" s="13" t="n">
         <v>0.02</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="10"/>
       <c r="C26" s="11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F26" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G26" s="13" t="n">
         <v>0.02</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="10"/>
       <c r="C27" s="11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F27" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G27" s="13" t="n">
         <v>0.02</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="10"/>
       <c r="C28" s="11" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G28" s="13" t="n">
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="10"/>
       <c r="C29" s="11" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F29" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F29" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G29" s="13" t="n">
         <v>0.02</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="10"/>
       <c r="C30" s="11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F30" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G30" s="13" t="n">
         <v>0.02</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="10"/>
       <c r="C31" s="11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="F31" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G31" s="13" t="n">
         <v>0.02</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="10"/>
       <c r="C32" s="11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="F32" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F32" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G32" s="13" t="n">
         <v>0.07</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="10"/>
       <c r="C33" s="11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="F33" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G33" s="13" t="n">
         <v>0.07</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="10"/>
       <c r="C34" s="11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F34" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F34" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G34" s="13" t="n">
         <v>0.02</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="10"/>
       <c r="C35" s="11" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F35" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F35" s="15" t="s">
         <v>11</v>
       </c>
       <c r="G35" s="13" t="n">
         <v>0.02</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C37" s="2" t="n">
         <f aca="false">SUM(G:G)</f>
         <v>8.27</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F6" r:id="rId1" display="Reichelt"/>

</xml_diff>